<commit_message>
Added HEX compilation date as parameter
</commit_message>
<xml_diff>
--- a/helpers/Analýza logov.xlsx
+++ b/helpers/Analýza logov.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\OVY\Staz\Analýza Logov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\log_analysis\log_analysis\src\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA06A3C1-580C-4CB3-BD8A-23FBB1B12CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E6D90F-D99A-46B8-AB00-3CEAE79927D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-8198" windowWidth="28995" windowHeight="15946" activeTab="2" xr2:uid="{275296B2-BD63-4ADD-8274-909CCA29756A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{275296B2-BD63-4ADD-8274-909CCA29756A}"/>
   </bookViews>
   <sheets>
     <sheet name="Poznámky" sheetId="3" r:id="rId1"/>
@@ -633,14 +633,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,7 +656,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -958,12 +958,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="171" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -971,13 +971,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -993,7 +993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1025,18 +1025,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -1058,14 +1058,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.81640625" customWidth="1"/>
+    <col min="3" max="3" width="81.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1092,25 +1092,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1142,27 +1142,27 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="1" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="36.28515625" customWidth="1"/>
+    <col min="10" max="10" width="36.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1180,14 +1180,14 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>671101</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>671101</v>
       </c>
@@ -1262,29 +1262,29 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1409,7 +1409,7 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1421,9 +1421,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1441,9 +1441,9 @@
       <selection activeCell="H32" sqref="H31:H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>46</v>
       </c>

</xml_diff>